<commit_message>
Backup QR Scanner data - 2025-12-08T18:47:27.028Z - Cache Bust: 1765219647028
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765192362295_f71267414ad928ff5abcafbc64a0ab66be7858c72295754f0460aad3fd95b393.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765192362295_f71267414ad928ff5abcafbc64a0ab66be7858c72295754f0460aad3fd95b393.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -439,7 +439,7 @@
         <v>Scan</v>
       </c>
       <c r="F2" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
         <v>Scan</v>
       </c>
       <c r="F3" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="4">
@@ -479,7 +479,7 @@
         <v>Scan</v>
       </c>
       <c r="F4" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="5">
@@ -499,7 +499,7 @@
         <v>Scan</v>
       </c>
       <c r="F5" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="6">
@@ -519,7 +519,7 @@
         <v>Scan</v>
       </c>
       <c r="F6" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="7">
@@ -539,7 +539,7 @@
         <v>Scan</v>
       </c>
       <c r="F7" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="8">
@@ -559,7 +559,7 @@
         <v>Scan</v>
       </c>
       <c r="F8" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="9">
@@ -579,7 +579,7 @@
         <v>Scan</v>
       </c>
       <c r="F9" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="10">
@@ -599,7 +599,7 @@
         <v>Scan</v>
       </c>
       <c r="F10" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="11">
@@ -619,7 +619,7 @@
         <v>Scan</v>
       </c>
       <c r="F11" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="12">
@@ -639,72 +639,12 @@
         <v>Manual</v>
       </c>
       <c r="F12" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>191076</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C13" t="str">
-        <v>08/12/2025</v>
-      </c>
-      <c r="D13" t="str">
-        <v>13:13:59</v>
-      </c>
-      <c r="E13" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F13" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>190795</v>
-      </c>
-      <c r="B14" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C14" t="str">
-        <v>08/12/2025</v>
-      </c>
-      <c r="D14" t="str">
-        <v>13:14:06</v>
-      </c>
-      <c r="E14" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F14" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>180752</v>
-      </c>
-      <c r="B15" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C15" t="str">
-        <v>08/12/2025</v>
-      </c>
-      <c r="D15" t="str">
-        <v>13:14:14</v>
-      </c>
-      <c r="E15" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F15" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>